<commit_message>
filegenerate 改名 界面调整 开始protobuff
</commit_message>
<xml_diff>
--- a/Assets/Code/Tools/QuickSheet/Example/Excel/Example.xlsx
+++ b/Assets/Code/Tools/QuickSheet/Example/Excel/Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GitHub\Unity-QuickSheet\Assets\QuickSheet\Example\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GitHub\R-Evolution\Assets\Code\Tools\QuickSheet\Example\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>Id</t>
   </si>
@@ -241,6 +241,22 @@
   </si>
   <si>
     <t>字符串分隔符[/]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>萨达</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>撒大声地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大萨达</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿萨德</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -811,241 +827,265 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="10" width="15.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="1" max="2" width="19.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="11" width="15.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="12.875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>212</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>4545</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.6</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>2312</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>33</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>545</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>777</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>44</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>212</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0.7</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>566</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>10</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0.22</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>45</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>22</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>0.66700000000000004</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>6945</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>43</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>1012</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>